<commit_message>
Timeline Assignment creation and other cases updation
</commit_message>
<xml_diff>
--- a/WebDriverMaven/src/test/resources/Data/excelWork.xlsx
+++ b/WebDriverMaven/src/test/resources/Data/excelWork.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="13665" windowHeight="2805" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15060" windowHeight="2775" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LandingPage" sheetId="1" r:id="rId1"/>
     <sheet name="HomePage" sheetId="2" r:id="rId2"/>
+    <sheet name="TimeLine" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:M7"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>FirstName</t>
   </si>
@@ -116,6 +118,12 @@
   </si>
   <si>
     <t>Gaurav Kumar Lal</t>
+  </si>
+  <si>
+    <t>PostText</t>
+  </si>
+  <si>
+    <t>Hello…</t>
   </si>
 </sst>
 </file>
@@ -674,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,4 +711,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>